<commit_message>
final modifications to the code
</commit_message>
<xml_diff>
--- a/nueva_solicitud_formato.xlsx
+++ b/nueva_solicitud_formato.xlsx
@@ -1,49 +1,101 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iteso01-my.sharepoint.com/personal/paulina_mejia_iteso_mx/Documents/9 SEMESTRE/MODELOS DE CRÉDITO/02_CreditModel_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_AABD3EFC984A5A4EE076ACB6554CB6F92ED7AA74" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3856CD9-3730-0E4E-A033-2FD5A00A7262}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_AABD917C1B7BEA8FE45BF8365D007EBC107BA295" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A928701-AAF2-8C45-98F9-06F19C9E0745}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="28480" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>INSTRUCCIONES: Llene una fila por cliente. No cambie el nombre NI el orden de las 8 columnas. Si un dato no aplica, ponga 0.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>Instrucciones: Reemplace los valores de ejemplo con los datos del nuevo cliente y guarde el archivo antes de ejecutar la FASE 11.</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>Annual_Income</t>
   </si>
   <si>
     <t>Monthly_Inhand_Salary</t>
   </si>
   <si>
+    <t>Num_Bank_Accounts</t>
+  </si>
+  <si>
+    <t>Num_Credit_Card</t>
+  </si>
+  <si>
+    <t>Interest_Rate</t>
+  </si>
+  <si>
+    <t>Num_of_Loan</t>
+  </si>
+  <si>
+    <t>Delay_from_due_date</t>
+  </si>
+  <si>
+    <t>Num_of_Delayed_Payment</t>
+  </si>
+  <si>
+    <t>Changed_Credit_Limit</t>
+  </si>
+  <si>
+    <t>Num_Credit_Inquiries</t>
+  </si>
+  <si>
+    <t>Credit_Mix</t>
+  </si>
+  <si>
+    <t>Outstanding_Debt</t>
+  </si>
+  <si>
+    <t>Credit_Utilization_Ratio</t>
+  </si>
+  <si>
+    <t>Credit_History_Age</t>
+  </si>
+  <si>
+    <t>Payment_of_Min_Amount</t>
+  </si>
+  <si>
     <t>Total_EMI_per_month</t>
   </si>
   <si>
-    <t>Credit_Utilization_Ratio</t>
-  </si>
-  <si>
-    <t>Credit_History_Age</t>
-  </si>
-  <si>
-    <t>Num_of_Delayed_Payment</t>
-  </si>
-  <si>
-    <t>Num_Credit_Inquiries</t>
-  </si>
-  <si>
-    <t>Outstanding_Debt</t>
+    <t>Amount_invested_monthly</t>
+  </si>
+  <si>
+    <t>Payment_Behaviour</t>
   </si>
   <si>
     <t>Monthly_Balance</t>
@@ -434,18 +486,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="173" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="186" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="20" customWidth="1"/>
+    <col min="1" max="21" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -456,8 +508,21 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -482,36 +547,202 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>480000</v>
+      </c>
+      <c r="D3">
         <v>40000</v>
       </c>
-      <c r="B3">
-        <v>2000</v>
-      </c>
-      <c r="C3">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <v>320</v>
-      </c>
       <c r="E3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>1300</v>
+        <v>12</v>
       </c>
       <c r="H3">
-        <v>4000</v>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
+      </c>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>28</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>2000</v>
+      </c>
+      <c r="S3">
+        <v>1500</v>
+      </c>
+      <c r="U3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>1080000</v>
+      </c>
+      <c r="D4">
+        <v>85000</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>15</v>
+      </c>
+      <c r="P4">
+        <v>220</v>
+      </c>
+      <c r="R4">
+        <v>3000</v>
+      </c>
+      <c r="S4">
+        <v>10000</v>
+      </c>
+      <c r="U4">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>180000</v>
+      </c>
+      <c r="D5">
+        <v>12000</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>65000</v>
+      </c>
+      <c r="O5">
+        <v>85</v>
+      </c>
+      <c r="P5">
+        <v>70</v>
+      </c>
+      <c r="R5">
+        <v>7000</v>
+      </c>
+      <c r="S5">
+        <v>200</v>
+      </c>
+      <c r="U5">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:U1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>